<commit_message>
update tool to private needs
</commit_message>
<xml_diff>
--- a/input/DbQuery_template.xlsx
+++ b/input/DbQuery_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thomas deter\Dateien\transfer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E25069CD-7FBB-4F80-9D8A-8BCC9CBBA1E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64474CA3-53BB-480A-9CBE-60366F8D2282}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -909,11 +909,13 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="14" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
+      <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
+      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -3836,9 +3838,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:AP50"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A58" sqref="A58"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -3860,10 +3860,7 @@
       <c r="B1" s="11" t="s">
         <v>217</v>
       </c>
-      <c r="F1" s="20">
-        <f ca="1">TODAY()</f>
-        <v>45555</v>
-      </c>
+      <c r="F1" s="20"/>
       <c r="G1" s="21"/>
       <c r="H1" s="21"/>
       <c r="I1" s="21"/>
@@ -6047,7 +6044,7 @@
       <c r="Y50" s="17"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="dEM71GNX94wz6OwR0uvWwU5AiwvFooQv8SC09LcwCxa2KZJ6MgahEXIHjzgku0jdAQthFlT9mLs3pxOZH79lWg==" saltValue="VRjWkkcTyB9QxaLhvaM8yw==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="fJ1iyNaxnB8gtI7tS/lFKIQR17GcbS1AQ/ARg+i06hm4lG28Pc3HA71OA2CtYoFFX4jGmb1p2b+Q9eAC7Ho6cQ==" saltValue="45NyrjTaRqidrGRFyZ9RUg==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="3">
     <mergeCell ref="F2:V33"/>
     <mergeCell ref="F35:V50"/>

</xml_diff>